<commit_message>
Corrected problems with rotation
</commit_message>
<xml_diff>
--- a/data/description_measures.xlsx
+++ b/data/description_measures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\covid-measures-uml\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B4BD4F-C520-49D0-BDFB-F95F658EFABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7400FC-86E8-4844-ACE6-E3F4FAD6BCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5172CFAE-47FF-456C-9827-2DDCBB3F67ED}"/>
   </bookViews>
@@ -96,16 +96,7 @@
     <t>H8_Protection of elderly people</t>
   </si>
   <si>
-    <t>measure</t>
-  </si>
-  <si>
-    <t>measure.minvalue</t>
-  </si>
-  <si>
     <t>measure.maxvalue</t>
-  </si>
-  <si>
-    <t>coding</t>
   </si>
   <si>
     <t>0 - no measures
@@ -228,12 +219,21 @@
 3 - Extensive restrictions for isolation and hygiene in LTCFs, all non-essential external visitors prohibited, and/or all elderly people required to stay at home and not leave the home with minimal exceptions, and receive no external visitors
 Blank - no data</t>
   </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,9 +242,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -263,20 +281,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,297 +636,301 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C4659F-9B02-4870-94F7-E415F72659BF}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="10.90625" style="2"/>
-    <col min="4" max="4" width="88.90625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.90625" style="2"/>
+    <col min="1" max="1" width="15.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="63.26953125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="91" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="104" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="87">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="78" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="87">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="65" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="91" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="58">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
+    </row>
+    <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="87">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="104" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
+    </row>
+    <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="58">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="87">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="130" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
+    </row>
+    <row r="21" spans="1:4" ht="130" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
         <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="58">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="87">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="72.5">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43.5">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="58">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.5">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="58">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="87">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.5">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.5">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.5">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="101.5">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="130.5">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="130.5">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>3</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>